<commit_message>
validado del lado del cliente
</commit_message>
<xml_diff>
--- a/ImportFiles/Proyectos_finales_informatica.xlsx
+++ b/ImportFiles/Proyectos_finales_informatica.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2490,7 +2490,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2592,7 +2592,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2627,7 +2627,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2804,7 +2804,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2814,7 +2814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F259" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2828,7 +2828,7 @@
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.140625" customWidth="1"/>
     <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="9" max="9" width="51.28515625" customWidth="1"/>
     <col min="10" max="10" width="31" customWidth="1"/>
     <col min="11" max="11" width="19.28515625" customWidth="1"/>
     <col min="12" max="12" width="19.5703125" customWidth="1"/>

</xml_diff>